<commit_message>
Working on compute times.
</commit_message>
<xml_diff>
--- a/computation times.xlsx
+++ b/computation times.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Kerk's laptop</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>BMsimGSSA</t>
+  </si>
+  <si>
+    <t>baseline2</t>
   </si>
 </sst>
 </file>
@@ -448,13 +451,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -499,165 +502,173 @@
         <v>20.870006689140801</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2">
-        <f>C4/C2</f>
-        <v>1.8518824345174754E-3</v>
-      </c>
-      <c r="C4">
-        <v>0.206367122009396</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>122.81623181398</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="B5" s="2">
+        <f>C5/C2</f>
+        <v>1.8518824345174754E-3</v>
+      </c>
+      <c r="C5">
+        <v>0.206367122009396</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2">
-        <f>D7/D2</f>
-        <v>31.537829729678734</v>
-      </c>
-      <c r="D7">
-        <v>3199.44684340299</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2">
-        <f>C8/C2</f>
-        <v>62.380262520635483</v>
-      </c>
-      <c r="C8">
-        <v>6951.4322327531399</v>
+        <f>D8/D2</f>
+        <v>31.537829729678734</v>
+      </c>
+      <c r="D8">
+        <v>3199.44684340299</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="2">
+        <f>C9/C2</f>
+        <v>62.380262520635483</v>
+      </c>
+      <c r="C9">
+        <v>6951.4322327531399</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2">
-        <f>C12/C2</f>
-        <v>9.1913275144513942E-5</v>
-      </c>
-      <c r="C12">
-        <v>1.0242485004710001E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <f>C13/C2</f>
+        <v>9.1913275144513942E-5</v>
+      </c>
+      <c r="C13">
+        <v>1.0242485004710001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1">
-        <f>F14/F2</f>
-        <v>2.9930979083545597</v>
-      </c>
-      <c r="F14">
-        <v>62.465973368613</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1">
-        <f>C15/C2</f>
-        <v>882.53140594451622</v>
-      </c>
-      <c r="C15">
-        <v>98346.127666106506</v>
+        <f>F15/F2</f>
+        <v>2.9930979083545597</v>
+      </c>
+      <c r="F15">
+        <v>62.465973368613</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B16" s="1">
+        <f>C16/C2</f>
+        <v>882.53140594451622</v>
+      </c>
+      <c r="C16">
+        <v>98346.127666106506</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="1">
-        <f>F17/F2</f>
+      <c r="B18" s="1">
+        <f>F18/F2</f>
         <v>595.22511766399043</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>12422.3521871921</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-    </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="2">
-        <f>D19/D2</f>
-        <v>1.2889469253580764E-3</v>
-      </c>
-      <c r="D19">
-        <v>0.130760968874471</v>
-      </c>
+      <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B20" s="2">
+        <f>D20/D2</f>
+        <v>1.2889469253580764E-3</v>
+      </c>
+      <c r="D20">
+        <v>0.130760968874471</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="1">
-        <f>D22/D2</f>
-        <v>21.322612219454879</v>
-      </c>
-      <c r="D22">
-        <v>2163.1343990180098</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B23" s="1">
+        <f>D23/D2</f>
+        <v>21.322612219454879</v>
+      </c>
+      <c r="D23">
+        <v>2163.1343990180098</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reorganizing and cleaning up folders
</commit_message>
<xml_diff>
--- a/computation times.xlsx
+++ b/computation times.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Kerk's laptop</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Kerk's desktop</t>
   </si>
   <si>
-    <t>Daryl's computer</t>
-  </si>
-  <si>
     <t>Relative</t>
   </si>
   <si>
@@ -104,6 +101,15 @@
   </si>
   <si>
     <t>baseline2</t>
+  </si>
+  <si>
+    <t>Anthony's desktop</t>
+  </si>
+  <si>
+    <t>Anthony's laptop</t>
+  </si>
+  <si>
+    <t>Daryl's laptop</t>
   </si>
 </sst>
 </file>
@@ -451,13 +457,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -465,9 +471,9 @@
     <col min="2" max="2" width="12.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -479,10 +485,16 @@
         <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -502,17 +514,20 @@
         <v>20.870006689140801</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3">
-        <v>122.81623181398</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>121.152892872923</v>
+      </c>
+      <c r="G3">
+        <v>104.580126871513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2">
         <f>C5/C2</f>
@@ -522,19 +537,19 @@
         <v>0.206367122009396</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2">
         <f>D8/D2</f>
@@ -544,9 +559,9 @@
         <v>3199.44684340299</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2">
         <f>C9/C2</f>
@@ -556,17 +571,17 @@
         <v>6951.4322327531399</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -578,12 +593,12 @@
         <v>1.0242485004710001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -595,7 +610,7 @@
         <v>62.465973368613</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>

</xml_diff>